<commit_message>
restore masterconfig and product json
</commit_message>
<xml_diff>
--- a/product/getProduct/products.xlsx
+++ b/product/getProduct/products.xlsx
@@ -763,17 +763,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>668c09bc30b0b830ec5cebed</t>
+          <t>6687b13c5a9fc761c43bcd1e</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'TRIAL': ['668c155630b0b830ec5cec0c'], 'PLATINUM': ['668c161b30b0b830ec5cec14'], 'GOLD': ['668c15e930b0b830ec5cec10', '668c15f330b0b830ec5cec11'], 'SILVER': ['668c15cb30b0b830ec5cec0f']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'GOLD': ['66d07c94b1dbc9702f40478e'], 'SILVER': ['668e18eb8205093c726fe448']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>IZAK</t>
+          <t>PI</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -788,17 +788,17 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Mobius</t>
+          <t>Mobius Pi is an advanced data lakehouse platform designed to offer robust data integration, processing, and analytics capabilities. It combines the best features of data warehouses and data lakes to provide a comprehensive solution for handling large-scale data operations, both transactional (OLTP) and analytical (OLAP).</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_232da7d6-008e-425f-9e57-fc2ae005e87d/ingestion/3c61245a-0302-434b-a192-2cb75a28cb4a_$$_V1_iZak%20logo.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/91dfc3e3-d66b-4218-b2f4-b226b1e06178_$$_V1_pi.png</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -813,7 +813,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>668c09bc30b0b830ec5cebec</t>
+          <t>6687b13c5a9fc761c43bcd1d</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -827,7 +827,7 @@
         </is>
       </c>
       <c r="N2" t="n">
-        <v>1720453564857</v>
+        <v>1720168764704</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -855,10 +855,10 @@
         </is>
       </c>
       <c r="T2" t="n">
-        <v>1720459236160</v>
+        <v>1727084089556</v>
       </c>
       <c r="U2" t="n">
-        <v>1720453564857</v>
+        <v>1720168764704</v>
       </c>
       <c r="V2" t="b">
         <v>1</v>
@@ -878,7 +878,7 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>232da7d6-008e-425f-9e57-fc2ae005e87d</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
@@ -1001,12 +1001,12 @@
       </c>
       <c r="BA2" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>{'data': [{'Description': 'PI offers codeless tools for visualizing data, making it easy to gain insights and make data-driven decisions.', 'imageUrl': 'assets/images/product/product view 22.png', 'Title': 'Data Visualisation'}, {'Description': 'PI supports all three layers of big data processing - ingest, process, and serve - enabling enterprises to unlock the full potential of their data.', 'imageUrl': 'assets/images/product/product view 27.png', 'Title': 'Big Data Processing'}, {'Description': 'PI provides tools for contextualising data and targeting specific groups, allowing businesses to personalise their offerings and improve customer experiences.', 'imageUrl': 'assets/images/product/product view 23.png', 'Title': 'Contextualisation and Targeting'}]}</t>
         </is>
       </c>
       <c r="BB2" t="inlineStr">
         <is>
-          <t>Portal.team@mobiusdtaas.ai</t>
+          <t>Mobius</t>
         </is>
       </c>
       <c r="BC2" t="inlineStr">
@@ -1015,20 +1015,20 @@
         </is>
       </c>
       <c r="BD2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BE2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF2" t="n">
         <v>0</v>
       </c>
       <c r="BG2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH2" t="inlineStr">
         <is>
-          <t>['AD_BASED', 'Paid']</t>
+          <t>['Paid', 'AD_BASED']</t>
         </is>
       </c>
       <c r="BI2" t="inlineStr">
@@ -1054,17 +1054,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>668c100c30b0b830ec5cebfc</t>
+          <t>668c0f2430b0b830ec5cebf9</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'TRIAL': ['668c172630b0b830ec5cec17'], 'PLATINUM': ['668c17c530b0b830ec5cec1a'], 'GOLD': ['668c178c30b0b830ec5cec19'], 'SILVER': ['668c175c30b0b830ec5cec18']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['668c187130b0b830ec5cec1b'], 'PLATINUM': ['668c18e830b0b830ec5cec1e'], 'GOLD': ['668c18c430b0b830ec5cec1d'], 'SILVER': ['668c189930b0b830ec5cec1c']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Slack</t>
+          <t>Youtube</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1079,7 +1079,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Slack is a communication platform designed for teams and workplaces. It offers real-time messaging, file sharing, and integrations with various tools and services. Users can create channels for different topics, direct message individuals, and collaborate seamlessly.</t>
+          <t>YouTube is a video-sharing platform where users can upload, watch, and share videos. Launched in 2005 and acquired by Google in 2006, it hosts a vast range of content, including music videos, tutorials, vlogs, and more. Users can subscribe to channels, comment on videos, and create playlists.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -1089,7 +1089,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://cdn.gov-cloud.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/3d41d17e-17b1-40c0-a729-8a439d7fc197_$$_V1_Slack_icon_2019.svg.png</t>
+          <t>https://cdn.gov-cloud.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/bdc8d020-62c6-4866-888d-a60572bd0bc4_$$_V1_YouTube-logo-vector-PNG.png</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -1104,7 +1104,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>668c100c30b0b830ec5cebfb</t>
+          <t>668c0f2430b0b830ec5cebf8</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -1118,7 +1118,7 @@
         </is>
       </c>
       <c r="N3" t="n">
-        <v>1720455180168</v>
+        <v>1720454948684</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -1146,10 +1146,10 @@
         </is>
       </c>
       <c r="T3" t="n">
-        <v>1723183206112</v>
+        <v>1724927989011</v>
       </c>
       <c r="U3" t="n">
-        <v>1720455180168</v>
+        <v>1720454948684</v>
       </c>
       <c r="V3" t="b">
         <v>1</v>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
@@ -1306,20 +1306,20 @@
         </is>
       </c>
       <c r="BD3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BE3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BF3" t="n">
         <v>0</v>
       </c>
       <c r="BG3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BH3" t="inlineStr">
         <is>
-          <t>['Paid', 'AD_BASED']</t>
+          <t>['AD_BASED', 'Paid']</t>
         </is>
       </c>
       <c r="BI3" t="inlineStr">
@@ -1345,17 +1345,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>668c13be30b0b830ec5cec07</t>
+          <t>668c100c30b0b830ec5cebfc</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['668c172630b0b830ec5cec17'], 'PLATINUM': ['668c17c530b0b830ec5cec1a'], 'GOLD': ['668c178c30b0b830ec5cec19'], 'SILVER': ['668c175c30b0b830ec5cec18']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Here Maps</t>
+          <t>Slack</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1370,7 +1370,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Engagements</t>
+          <t>Slack is a communication platform designed for teams and workplaces. It offers real-time messaging, file sharing, and integrations with various tools and services. Users can create channels for different topics, direct message individuals, and collaborate seamlessly.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -1380,7 +1380,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://cdn.gov-cloud.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/3acd11c3-50a8-423b-87e3-feed87f1cd7e_$$_V1_here%20maps.png</t>
+          <t>https://cdn.gov-cloud.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/3d41d17e-17b1-40c0-a729-8a439d7fc197_$$_V1_Slack_icon_2019.svg.png</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -1395,7 +1395,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>668c13be30b0b830ec5cec06</t>
+          <t>668c100c30b0b830ec5cebfb</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -1409,7 +1409,7 @@
         </is>
       </c>
       <c r="N4" t="n">
-        <v>1720456126864</v>
+        <v>1720455180168</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -1437,10 +1437,10 @@
         </is>
       </c>
       <c r="T4" t="n">
-        <v>1723179338157</v>
+        <v>1723183206112</v>
       </c>
       <c r="U4" t="n">
-        <v>1720456126864</v>
+        <v>1720455180168</v>
       </c>
       <c r="V4" t="b">
         <v>1</v>
@@ -1460,7 +1460,7 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
@@ -1636,17 +1636,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>668e83dcc8fea21f886ddd4e</t>
+          <t>668c1d7430b0b830ec5cec24</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba113efefec82e4820d272', '66e3dcfe83d08979e96cef14'], 'PLATINUM': ['66ba113efefec82e4820d274', '66e3dd0083d08979e96cef15'], 'GOLD': ['66ba113e9ef55a4cad1e1361', '66e3dcffb1dbc9702f40497a'], 'SILVER': ['66ba113efefec82e4820d273', '66e3dcffb1dbc9702f404979']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Trigger Workflow</t>
+          <t>WhatsApp</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>This product is used to trigger the next workflow.</t>
+          <t xml:space="preserve">WhatsApp is a messaging app that allows users to send text messages, voice messages, make voice and video calls, and share images, documents, and other media. </t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1669,7 +1669,11 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://cdn.gov-cloud.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/847a9003-06bf-4097-a90d-80936cfed99d_$$_V1_whatsapp.png</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>['OTT', 'DATA CASTING']</t>
@@ -1682,7 +1686,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>668e83dcc8fea21f886ddd4d</t>
+          <t>668c1d7430b0b830ec5cec23</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -1696,7 +1700,7 @@
         </is>
       </c>
       <c r="N5" t="n">
-        <v>1720615900574</v>
+        <v>1720458612036</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1724,10 +1728,10 @@
         </is>
       </c>
       <c r="T5" t="n">
-        <v>1721999307423</v>
+        <v>1723179529824</v>
       </c>
       <c r="U5" t="n">
-        <v>1720615900574</v>
+        <v>1720458612036</v>
       </c>
       <c r="V5" t="b">
         <v>1</v>
@@ -1747,7 +1751,7 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
@@ -1890,14 +1894,14 @@
         <v>0</v>
       </c>
       <c r="BF5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG5" t="n">
         <v>0</v>
       </c>
       <c r="BH5" t="inlineStr">
         <is>
-          <t>['AD_BASED', 'Paid']</t>
+          <t>['Paid', 'AD_BASED']</t>
         </is>
       </c>
       <c r="BI5" t="inlineStr">
@@ -1923,17 +1927,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>6675217b72fb483cdd3be10a</t>
+          <t>668c0ac630b0b830ec5cebf1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['668c244630b0b830ec5cec42'], 'PLATINUM': ['668c243c30b0b830ec5cec41'], 'GOLD': ['668c245530b0b830ec5cec44'], 'SILVER': ['668c244d30b0b830ec5cec43']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Product_negotiation_testing3</t>
+          <t>Kepler</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1948,7 +1952,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>weather service provider</t>
+          <t>Mobius</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1958,7 +1962,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://cdn.jim-nielsen.com/ios/512/weather-2021-12-07.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_232da7d6-008e-425f-9e57-fc2ae005e87d/ingestion/895e36f0-c59d-4626-9e40-62ea55a3e15d_$$_V1_Kepler.png</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -1973,7 +1977,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>6675217b72fb483cdd3be109</t>
+          <t>668c0ac630b0b830ec5cebf0</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -1987,7 +1991,7 @@
         </is>
       </c>
       <c r="N6" t="n">
-        <v>1718952315550</v>
+        <v>1720453830929</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -2015,10 +2019,10 @@
         </is>
       </c>
       <c r="T6" t="n">
-        <v>1721999006553</v>
+        <v>1720459650985</v>
       </c>
       <c r="U6" t="n">
-        <v>1718952315550</v>
+        <v>1720453830929</v>
       </c>
       <c r="V6" t="b">
         <v>1</v>
@@ -2038,7 +2042,7 @@
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
@@ -2166,7 +2170,7 @@
       </c>
       <c r="BB6" t="inlineStr">
         <is>
-          <t>Mobius Mobius</t>
+          <t>Portal.team@mobiusdtaas.ai</t>
         </is>
       </c>
       <c r="BC6" t="inlineStr">
@@ -2175,16 +2179,16 @@
         </is>
       </c>
       <c r="BD6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BE6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BF6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BG6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH6" t="inlineStr">
         <is>
@@ -2214,17 +2218,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6687b13c5a9fc761c43bcd1e</t>
+          <t>668c2e3730b0b830ec5cec4e</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'SILVER': ['668e18eb8205093c726fe448']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba10ed9ef55a4cad1e1346'], 'PLATINUM': ['66ba10edfefec82e4820d25a'], 'GOLD': ['66ba10ed9ef55a4cad1e1347', '66d084c9b1dbc9702f40479f'], 'SILVER': ['66ba10edfefec82e4820d259']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PI</t>
+          <t>VoteIQ</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2239,17 +2243,17 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Mobius Pi is an advanced data lakehouse platform designed to offer robust data integration, processing, and analytics capabilities. It combines the best features of data warehouses and data lakes to provide a comprehensive solution for handling large-scale data operations, both transactional (OLTP) and analytical (OLAP).</t>
+          <t>VoteIQ revolutionizes local governance by enabling citizens to participate in Panchayat Raj, manage cooperative services, and handle home-related tasks directly from their smart devices. This app empowers citizens to engage with their local government seamlessly, ensuring democratic processes are more accessible and participatory, ultimately strengthening community involvement and transparency in governance.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>XP</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/91dfc3e3-d66b-4218-b2f4-b226b1e06178_$$_V1_pi.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/68b498cc-12ad-4b3e-b17e-114bccae6cb3_$$_V1_voteiq.png</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -2264,7 +2268,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>6687b13c5a9fc761c43bcd1d</t>
+          <t>668c2e3730b0b830ec5cec4d</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -2278,7 +2282,7 @@
         </is>
       </c>
       <c r="N7" t="n">
-        <v>1720168764704</v>
+        <v>1720462903816</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -2306,10 +2310,10 @@
         </is>
       </c>
       <c r="T7" t="n">
-        <v>1722922334356</v>
+        <v>1720530450272</v>
       </c>
       <c r="U7" t="n">
-        <v>1720168764704</v>
+        <v>1720462903816</v>
       </c>
       <c r="V7" t="b">
         <v>1</v>
@@ -2329,7 +2333,7 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
@@ -2452,12 +2456,12 @@
       </c>
       <c r="BA7" t="inlineStr">
         <is>
-          <t>{'data': [{'Description': 'PI offers codeless tools for visualizing data, making it easy to gain insights and make data-driven decisions.', 'imageUrl': 'assets/images/product/product view 22.png', 'Title': 'Data Visualisation'}, {'Description': 'PI supports all three layers of big data processing - ingest, process, and serve - enabling enterprises to unlock the full potential of their data.', 'imageUrl': 'assets/images/product/product view 27.png', 'Title': 'Big Data Processing'}, {'Description': 'PI provides tools for contextualising data and targeting specific groups, allowing businesses to personalise their offerings and improve customer experiences.', 'imageUrl': 'assets/images/product/product view 23.png', 'Title': 'Contextualisation and Targeting'}]}</t>
+          <t>{}</t>
         </is>
       </c>
       <c r="BB7" t="inlineStr">
         <is>
-          <t>Mobius</t>
+          <t>Mobius Mobius</t>
         </is>
       </c>
       <c r="BC7" t="inlineStr">
@@ -2466,20 +2470,20 @@
         </is>
       </c>
       <c r="BD7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BE7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF7" t="n">
         <v>0</v>
       </c>
       <c r="BG7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH7" t="inlineStr">
         <is>
-          <t>['Paid', 'AD_BASED']</t>
+          <t>['AD_BASED', 'Paid']</t>
         </is>
       </c>
       <c r="BI7" t="inlineStr">
@@ -2505,17 +2509,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>668c30cb30b0b830ec5cec56</t>
+          <t>668c113e30b0b830ec5cec00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['668c236b30b0b830ec5cec2e', '668c237330b0b830ec5cec2f'], 'PLATINUM': ['668c239130b0b830ec5cec32'], 'GOLD': ['668c238a30b0b830ec5cec31'], 'SILVER': ['668c237f30b0b830ec5cec30']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Museo</t>
+          <t>The weather-company</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -2530,17 +2534,17 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Museo promotes handloom and textile sectors by offering artisans a platform to showcase their work, access markets, and receive government support. This app helps traditional crafts thrive, enriching cultural heritage and boosting economic opportunities for artisans. It preserves and promotes these crafts, ensuring their continued significance in modern society</t>
+          <t>Mobius</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>XP</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/b879c7bc-07ba-452f-a1b2-f1bce80ea80d_$$_V1_Screenshot%20from%202024-07-09%2000-02-35.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/6a845d87-712e-4589-b015-427a40ef6144_$$_V1_The%20company%20wether.png</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -2555,7 +2559,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>668c30cb30b0b830ec5cec55</t>
+          <t>668c113e30b0b830ec5cebff</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -2569,7 +2573,7 @@
         </is>
       </c>
       <c r="N8" t="n">
-        <v>1720463563479</v>
+        <v>1720455486157</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -2597,10 +2601,10 @@
         </is>
       </c>
       <c r="T8" t="n">
-        <v>1720463563479</v>
+        <v>1722328270441</v>
       </c>
       <c r="U8" t="n">
-        <v>1720463563479</v>
+        <v>1720455486157</v>
       </c>
       <c r="V8" t="b">
         <v>1</v>
@@ -2620,7 +2624,7 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr">
@@ -2770,7 +2774,7 @@
       </c>
       <c r="BH8" t="inlineStr">
         <is>
-          <t>['AD_BASED', 'Paid']</t>
+          <t>['Paid', 'AD_BASED']</t>
         </is>
       </c>
       <c r="BI8" t="inlineStr">
@@ -2796,17 +2800,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>668c0f2430b0b830ec5cebf9</t>
+          <t>66950496b8561e10d7e5d437</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'TRIAL': ['668c187130b0b830ec5cec1b'], 'PLATINUM': ['668c18e830b0b830ec5cec1e'], 'GOLD': ['668c18c430b0b830ec5cec1d'], 'SILVER': ['668c189930b0b830ec5cec1c']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Youtube</t>
+          <t>ONDC</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2821,7 +2825,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>YouTube is a video-sharing platform where users can upload, watch, and share videos. Launched in 2005 and acquired by Google in 2006, it hosts a vast range of content, including music videos, tutorials, vlogs, and more. Users can subscribe to channels, comment on videos, and create playlists.</t>
+          <t>Open Network for Digital Commerce, is a private non-profit Section 8 company established by the Department for Promotion of Industry and Internal Trade of Government of India to develop open e-commerce</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -2829,11 +2833,7 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>https://cdn.gov-cloud.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/bdc8d020-62c6-4866-888d-a60572bd0bc4_$$_V1_YouTube-logo-vector-PNG.png</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
           <t>['OTT', 'DATA CASTING']</t>
@@ -2846,7 +2846,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>668c0f2430b0b830ec5cebf8</t>
+          <t>66950496b8561e10d7e5d436</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -2860,7 +2860,7 @@
         </is>
       </c>
       <c r="N9" t="n">
-        <v>1720454948684</v>
+        <v>1721042070451</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -2888,10 +2888,10 @@
         </is>
       </c>
       <c r="T9" t="n">
-        <v>1723179562287</v>
+        <v>1721196779341</v>
       </c>
       <c r="U9" t="n">
-        <v>1720454948684</v>
+        <v>1721042070451</v>
       </c>
       <c r="V9" t="b">
         <v>1</v>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA9" t="inlineStr">
@@ -3087,17 +3087,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>668c0e7b30b0b830ec5cebf7</t>
+          <t>668c31fd30b0b830ec5cec5a</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba114dfefec82e4820d286'], 'PLATINUM': ['66ba114efefec82e4820d288'], 'GOLD': ['66ba114d9ef55a4cad1e1379'], 'SILVER': ['66ba114dfefec82e4820d287']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>WHUT - TV</t>
+          <t>HearHere</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -3112,17 +3112,17 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Mobius</t>
+          <t>Hear, Here excels in marketing and public relations, ensuring citizens are aware of government services and benefits. It enhances the visibility and outreach of government programs through strategic communication efforts. This app keeps citizens informed and engaged, making government initiatives accessible and well-publicized</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>XP</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://cdn.gov-cloud.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/d1c36a1d-f5bf-47ce-afbb-8811e5b51f1c_$$_V1_mhut-tv.png</t>
+          <t>https://cdn.gov-cloud.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/6804a1a8-2a92-4bde-88f4-56afb61ccae0_$$_V1_here%20here.png</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -3137,7 +3137,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>668c0e7b30b0b830ec5cebf6</t>
+          <t>668c31fd30b0b830ec5cec59</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -3151,7 +3151,7 @@
         </is>
       </c>
       <c r="N10" t="n">
-        <v>1720454779274</v>
+        <v>1720463869655</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -3179,10 +3179,10 @@
         </is>
       </c>
       <c r="T10" t="n">
-        <v>1723184825345</v>
+        <v>1723179358214</v>
       </c>
       <c r="U10" t="n">
-        <v>1720454779274</v>
+        <v>1720463869655</v>
       </c>
       <c r="V10" t="b">
         <v>1</v>
@@ -3202,7 +3202,7 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr">
@@ -3352,7 +3352,7 @@
       </c>
       <c r="BH10" t="inlineStr">
         <is>
-          <t>['AD_BASED', 'Paid']</t>
+          <t>['Paid', 'AD_BASED']</t>
         </is>
       </c>
       <c r="BI10" t="inlineStr">
@@ -3378,17 +3378,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>668c333430b0b830ec5cec60</t>
+          <t>668c30cb30b0b830ec5cec56</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba10eafefec82e4820d253'], 'PLATINUM': ['66ba10ea9ef55a4cad1e1342', '66d084c8b1dbc9702f40479d'], 'GOLD': ['66ba10ea9ef55a4cad1e1341'], 'SILVER': ['66ba10ea9ef55a4cad1e1340']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Voxa</t>
+          <t>Museo</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -3403,7 +3403,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Voxa markets government services across public and private platforms. Collaborating with Information, Public Relations, and Marketing departments, it ensures widespread awareness and engagement. Voxa leverages multiple channels to maximize the reach and impact of government programs, fostering public awareness and encouraging citizen participation in services.</t>
+          <t>Museo promotes handloom and textile sectors by offering artisans a platform to showcase their work, access markets, and receive government support. This app helps traditional crafts thrive, enriching cultural heritage and boosting economic opportunities for artisans. It preserves and promotes these crafts, ensuring their continued significance in modern society</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/4bc5cb52-d6be-43f2-9ddc-2c6a9ec9fbed_$$_V1_Screenshot%20from%202024-07-09%2000-12-54.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/b879c7bc-07ba-452f-a1b2-f1bce80ea80d_$$_V1_Screenshot%20from%202024-07-09%2000-02-35.png</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -3428,7 +3428,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>668c333430b0b830ec5cec5f</t>
+          <t>668c30cb30b0b830ec5cec55</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -3442,7 +3442,7 @@
         </is>
       </c>
       <c r="N11" t="n">
-        <v>1720464180041</v>
+        <v>1720463563479</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -3470,10 +3470,10 @@
         </is>
       </c>
       <c r="T11" t="n">
-        <v>1720464180041</v>
+        <v>1720463563479</v>
       </c>
       <c r="U11" t="n">
-        <v>1720464180041</v>
+        <v>1720463563479</v>
       </c>
       <c r="V11" t="b">
         <v>1</v>
@@ -3493,7 +3493,7 @@
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA11" t="inlineStr">
@@ -3669,17 +3669,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>668c29a230b0b830ec5cec48</t>
+          <t>668c0a2430b0b830ec5cebef</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'PLATINUM': ['66b3585bfefec82e4820d23d'], 'GOLD': ['66b358129ef55a4cad1e132a'], 'SILVER': ['66b357d09ef55a4cad1e1329']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba1149fefec82e4820d27f'], 'PLATINUM': ['66ba114a9ef55a4cad1e1371'], 'GOLD': ['66ba114a9ef55a4cad1e1370'], 'SILVER': ['66ba1149fefec82e4820d280']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MXaaS</t>
+          <t>Tomorrow.io</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3694,17 +3694,17 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Marketplace as a Service</t>
+          <t>Mobius</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>XP</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>jjuuhyhg</t>
+          <t>https://cdn.mobiusdtaas.ai//_232da7d6-008e-425f-9e57-fc2ae005e87d/ingestion/5f70aae8-e024-4b83-a450-0bdc50b26c6d_$$_V1_tomarrow.io.png</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -3719,7 +3719,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>668c29a230b0b830ec5cec47</t>
+          <t>668c0a2430b0b830ec5cebee</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -3733,7 +3733,7 @@
         </is>
       </c>
       <c r="N12" t="n">
-        <v>1720461730788</v>
+        <v>1720453668236</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -3761,10 +3761,10 @@
         </is>
       </c>
       <c r="T12" t="n">
-        <v>1720529910436</v>
+        <v>1720459606021</v>
       </c>
       <c r="U12" t="n">
-        <v>1720461730788</v>
+        <v>1720453668236</v>
       </c>
       <c r="V12" t="b">
         <v>1</v>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA12" t="inlineStr">
@@ -3912,7 +3912,7 @@
       </c>
       <c r="BB12" t="inlineStr">
         <is>
-          <t>Mobius Mobius</t>
+          <t>Portal.team@mobiusdtaas.ai</t>
         </is>
       </c>
       <c r="BC12" t="inlineStr">
@@ -3927,7 +3927,7 @@
         <v>0</v>
       </c>
       <c r="BF12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG12" t="n">
         <v>0</v>
@@ -3960,17 +3960,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>668c2e3730b0b830ec5cec4e</t>
+          <t>668c32eb30b0b830ec5cec5e</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba1134fefec82e4820d25d'], 'PLATINUM': ['66ba11349ef55a4cad1e134b'], 'GOLD': ['66ba1134fefec82e4820d25e'], 'SILVER': ['66ba11349ef55a4cad1e134a']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>VoteIQ</t>
+          <t>SuperDashboard</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3985,7 +3985,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>VoteIQ revolutionizes local governance by enabling citizens to participate in Panchayat Raj, manage cooperative services, and handle home-related tasks directly from their smart devices. This app empowers citizens to engage with their local government seamlessly, ensuring democratic processes are more accessible and participatory, ultimately strengthening community involvement and transparency in governance.</t>
+          <t>The Super Dashboard monitors government services performance. Offering real-time insights and analytics, it helps nodal officers track effectiveness and efficiency. Super Dashboard empowers officials to make data-driven decisions and optimize public service delivery.</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -3995,7 +3995,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/68b498cc-12ad-4b3e-b17e-114bccae6cb3_$$_V1_voteiq.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/7a673b4f-334d-4439-884a-cf768838a178_$$_V1_Screenshot%20from%202024-07-09%2000-11-24.png</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -4010,7 +4010,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>668c2e3730b0b830ec5cec4d</t>
+          <t>668c32eb30b0b830ec5cec5d</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -4024,7 +4024,7 @@
         </is>
       </c>
       <c r="N13" t="n">
-        <v>1720462903816</v>
+        <v>1720464107519</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -4052,10 +4052,10 @@
         </is>
       </c>
       <c r="T13" t="n">
-        <v>1720530450272</v>
+        <v>1720464107519</v>
       </c>
       <c r="U13" t="n">
-        <v>1720462903816</v>
+        <v>1720464107519</v>
       </c>
       <c r="V13" t="b">
         <v>1</v>
@@ -4075,7 +4075,7 @@
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA13" t="inlineStr">
@@ -4251,17 +4251,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>6694b76bc8fea21f886ddd65</t>
+          <t>668c2fce30b0b830ec5cec52</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba114a9ef55a4cad1e1372'], 'PLATINUM': ['66ba114bfefec82e4820d281'], 'GOLD': ['66ba114b9ef55a4cad1e1374'], 'SILVER': ['66ba114a9ef55a4cad1e1373']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>FastApi</t>
+          <t>ImpressIO</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -4276,17 +4276,17 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>mobius</t>
+          <t>Impressio turns everyday objects into dynamic communication tools. It transforms highway signs into real-time incident alerts and local ad spaces into weather update platforms. This flexibility ensures citizens receive timely, relevant information through various channels, enhancing public communication and keeping the community informed and safe.</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>XP</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/9d56fb82-a1c4-4f64-a812-6798527c541b_$$_V1_fastapiimg.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/5b8bf081-031d-44dc-b2a4-8bb864736761_$$_V1_Frame.png</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -4301,7 +4301,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>6694b76bc8fea21f886ddd64</t>
+          <t>668c2fce30b0b830ec5cec51</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -4315,7 +4315,7 @@
         </is>
       </c>
       <c r="N14" t="n">
-        <v>1721022315726</v>
+        <v>1720463310070</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -4343,10 +4343,10 @@
         </is>
       </c>
       <c r="T14" t="n">
-        <v>1721299640241</v>
+        <v>1720528832394</v>
       </c>
       <c r="U14" t="n">
-        <v>1721022315726</v>
+        <v>1720463310070</v>
       </c>
       <c r="V14" t="b">
         <v>1</v>
@@ -4366,7 +4366,7 @@
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA14" t="inlineStr">
@@ -4516,7 +4516,7 @@
       </c>
       <c r="BH14" t="inlineStr">
         <is>
-          <t>['Paid', 'AD_BASED']</t>
+          <t>['AD_BASED', 'Paid']</t>
         </is>
       </c>
       <c r="BI14" t="inlineStr">
@@ -4542,17 +4542,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>668c32eb30b0b830ec5cec5e</t>
+          <t>668c337f30b0b830ec5cec62</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba11419ef55a4cad1e1365'], 'PLATINUM': ['66ba11419ef55a4cad1e1367'], 'GOLD': ['66ba11419ef55a4cad1e1366'], 'SILVER': ['66ba1141fefec82e4820d27a']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>SuperDashboard</t>
+          <t>Marco</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -4567,7 +4567,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>The Super Dashboard monitors government services performance. Offering real-time insights and analytics, it helps nodal officers track effectiveness and efficiency. Super Dashboard empowers officials to make data-driven decisions and optimize public service delivery.</t>
+          <t>Marco models the impact, economics, costs, and revenues of government services. Supporting Finance departments and nodal officers, it provides critical insights for financial planning and decision-making. Marco offers economic models and cost-benefit analyses, helping governments optimize resource allocation and enhance sustainability.</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -4577,7 +4577,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/7a673b4f-334d-4439-884a-cf768838a178_$$_V1_Screenshot%20from%202024-07-09%2000-11-24.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/3ec11f81-13ce-4d0a-a134-4d20e9f4088d_$$_V1_Screenshot%20from%202024-07-09%2000-14-03.png</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -4592,7 +4592,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>668c32eb30b0b830ec5cec5d</t>
+          <t>668c337f30b0b830ec5cec61</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -4606,7 +4606,7 @@
         </is>
       </c>
       <c r="N15" t="n">
-        <v>1720464107519</v>
+        <v>1720464255234</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -4634,10 +4634,10 @@
         </is>
       </c>
       <c r="T15" t="n">
-        <v>1720464107519</v>
+        <v>1720464255234</v>
       </c>
       <c r="U15" t="n">
-        <v>1720464107519</v>
+        <v>1720464255234</v>
       </c>
       <c r="V15" t="b">
         <v>1</v>
@@ -4657,7 +4657,7 @@
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA15" t="inlineStr">
@@ -4833,17 +4833,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>66962d7eb8561e10d7e5d439</t>
+          <t>668c1c7730b0b830ec5cec22</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba113f9ef55a4cad1e1362'], 'PLATINUM': ['66ba113ffefec82e4820d275'], 'GOLD': ['66ba113f9ef55a4cad1e1364'], 'SILVER': ['66ba113f9ef55a4cad1e1363']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>D2D ATSC3</t>
+          <t>Instagram</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -4858,7 +4858,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>  </t>
+          <t>Instagram is a social media platform for sharing photos and videos. Launched in 2010 and acquired by Facebook in 2012, it allows users to post visual content, follow accounts, and interact through likes, comments, and direct messages. Features include stories, reels, and various editing tools.</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -4866,7 +4866,11 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/5b1c33cc-0f06-48a7-b8a7-dfe6f9d9188e_$$_V1_instagram-logo-png-transparent-background.png</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr">
         <is>
           <t>['OTT', 'DATA CASTING']</t>
@@ -4879,7 +4883,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>66962d7eb8561e10d7e5d438</t>
+          <t>668c1c7730b0b830ec5cec21</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -4893,7 +4897,7 @@
         </is>
       </c>
       <c r="N16" t="n">
-        <v>1721118078705</v>
+        <v>1720458359494</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -4921,10 +4925,10 @@
         </is>
       </c>
       <c r="T16" t="n">
-        <v>1721202169624</v>
+        <v>1720530050313</v>
       </c>
       <c r="U16" t="n">
-        <v>1721118078705</v>
+        <v>1720458359494</v>
       </c>
       <c r="V16" t="b">
         <v>1</v>
@@ -4944,7 +4948,7 @@
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA16" t="inlineStr">
@@ -5120,17 +5124,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>668c315030b0b830ec5cec58</t>
+          <t>66962d7eb8561e10d7e5d439</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba11359ef55a4cad1e134c'], 'PLATINUM': ['66ba1135fefec82e4820d260'], 'GOLD': ['66ba1135fefec82e4820d25f'], 'SILVER': ['66ba11359ef55a4cad1e134d']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>D2D ATSC3</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -5145,19 +5149,15 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Mo ensures government messages reach the public effectively through diverse communication channels. It fosters transparency and engagement by keeping citizens informed about government announcements and updates. This app strengthens the relationship between the government and citizens, enhancing trust and ensuring that important information is widely disseminated.</t>
+          <t>  </t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>XP</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/0936f6ff-61bb-44ef-9223-b2ed7c0eb99a_$$_V1_mooooocolour%201.png</t>
-        </is>
-      </c>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
           <t>['OTT', 'DATA CASTING']</t>
@@ -5170,7 +5170,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>668c315030b0b830ec5cec57</t>
+          <t>66962d7eb8561e10d7e5d438</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -5184,7 +5184,7 @@
         </is>
       </c>
       <c r="N17" t="n">
-        <v>1720463696381</v>
+        <v>1721118078705</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -5212,10 +5212,10 @@
         </is>
       </c>
       <c r="T17" t="n">
-        <v>1720530513525</v>
+        <v>1721202169624</v>
       </c>
       <c r="U17" t="n">
-        <v>1720463696381</v>
+        <v>1721118078705</v>
       </c>
       <c r="V17" t="b">
         <v>1</v>
@@ -5235,7 +5235,7 @@
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA17" t="inlineStr">
@@ -5385,7 +5385,7 @@
       </c>
       <c r="BH17" t="inlineStr">
         <is>
-          <t>['AD_BASED', 'Paid']</t>
+          <t>['Paid', 'AD_BASED']</t>
         </is>
       </c>
       <c r="BI17" t="inlineStr">
@@ -5411,17 +5411,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>668c092b30b0b830ec5cebeb</t>
+          <t>668c0b2730b0b830ec5cebf3</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'TRIAL': ['668c13a830b0b830ec5cec05'], 'PLATINUM': ['668c145e30b0b830ec5cec0a', '668c231f30b0b830ec5cec2a'], 'GOLD': ['668c142530b0b830ec5cec09', '668c148630b0b830ec5cec0b'], 'SILVER': ['668c140630b0b830ec5cec08']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba11389ef55a4cad1e1357'], 'PLATINUM': ['66ba1139fefec82e4820d266'], 'GOLD': ['66ba1139fefec82e4820d265'], 'SILVER': ['66ba1139fefec82e4820d264']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Aegis</t>
+          <t>Facebook</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -5436,17 +5436,17 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Mobius</t>
+          <t>Facebook is a social media platform founded by Mark Zuckerberg in 2004. It allows users to create profiles, share photos and videos, send messages, and stay connected with friends and family. Users can also join groups, follow pages, and participate in events.</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>CP</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_232da7d6-008e-425f-9e57-fc2ae005e87d/ingestion/e4691f05-144c-48d1-bbe5-d0348cd3288a_$$_V1_aegis_logo%202.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/e1671c2a-85bc-49ee-9462-b2fa8bbb6fb6_$$_V1_facebook.png</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -5461,7 +5461,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>668c092b30b0b830ec5cebea</t>
+          <t>668c0b2730b0b830ec5cebf2</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -5475,7 +5475,7 @@
         </is>
       </c>
       <c r="N18" t="n">
-        <v>1720453419781</v>
+        <v>1720453927270</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -5503,10 +5503,10 @@
         </is>
       </c>
       <c r="T18" t="n">
-        <v>1723113530476</v>
+        <v>1721999294985</v>
       </c>
       <c r="U18" t="n">
-        <v>1720453419781</v>
+        <v>1720453927270</v>
       </c>
       <c r="V18" t="b">
         <v>1</v>
@@ -5526,7 +5526,7 @@
       </c>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>232da7d6-008e-425f-9e57-fc2ae005e87d</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA18" t="inlineStr">
@@ -5654,7 +5654,7 @@
       </c>
       <c r="BB18" t="inlineStr">
         <is>
-          <t>Portal.team@mobiusdtaas.ai</t>
+          <t>Mobius Mobius</t>
         </is>
       </c>
       <c r="BC18" t="inlineStr">
@@ -5663,16 +5663,16 @@
         </is>
       </c>
       <c r="BD18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BE18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BF18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BG18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH18" t="inlineStr">
         <is>
@@ -5702,17 +5702,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>668c33e030b0b830ec5cec64</t>
+          <t>668c342030b0b830ec5cec66</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba113a9ef55a4cad1e135a'], 'PLATINUM': ['66ba113bfefec82e4820d26a'], 'GOLD': ['66ba113bfefec82e4820d269'], 'SILVER': ['66ba113a9ef55a4cad1e135b']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Quirto</t>
+          <t>CX Delight</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -5727,7 +5727,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>TedaaS integrates gamification, rewards, and incentives to promote government services adoption. Collaborating with nodal officers and program secretaries, it designs engaging frameworks to encourage citizen participation. TedaaS enhances user engagement and drives higher adoption rates for public programs.</t>
+          <t>CX Delight customizes Mobius applications by region and operator, ensuring tailored user experiences. It enhances service delivery and satisfaction by providing localized interfaces. CX Delight makes government services more relevant and user-friendly for diverse communities.</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -5737,7 +5737,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/b6c0370b-9411-40ba-b838-3c47e548f7fa_$$_V1_Screenshot%20from%202024-07-09%2000-15-38.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/1b910183-8398-4e8e-b856-e86e7195629c_$$_V1_Screenshot%20from%202024-07-09%2000-16-52.png</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -5752,7 +5752,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>668c33e030b0b830ec5cec63</t>
+          <t>668c342030b0b830ec5cec65</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -5766,7 +5766,7 @@
         </is>
       </c>
       <c r="N19" t="n">
-        <v>1720464352686</v>
+        <v>1720464416284</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -5794,10 +5794,10 @@
         </is>
       </c>
       <c r="T19" t="n">
-        <v>1721998105721</v>
+        <v>1720464416284</v>
       </c>
       <c r="U19" t="n">
-        <v>1720464352686</v>
+        <v>1720464416284</v>
       </c>
       <c r="V19" t="b">
         <v>1</v>
@@ -5817,7 +5817,7 @@
       </c>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA19" t="inlineStr">
@@ -5993,17 +5993,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>668e66804b755826842e2741</t>
+          <t>668c092b30b0b830ec5cebeb</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'PLATINUM': ['668e6c784b755826842e2745', '668e6cbc4b755826842e2746']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['668c13a830b0b830ec5cec05'], 'PLATINUM': ['668c145e30b0b830ec5cec0a', '668c231f30b0b830ec5cec2a'], 'GOLD': ['668c142530b0b830ec5cec09', '668c148630b0b830ec5cec0b'], 'SILVER': ['668c140630b0b830ec5cec08']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>PI</t>
+          <t>Aegis</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -6023,12 +6023,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>CP</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>jjuuhyhg</t>
+          <t>https://cdn.mobiusdtaas.ai//_232da7d6-008e-425f-9e57-fc2ae005e87d/ingestion/e4691f05-144c-48d1-bbe5-d0348cd3288a_$$_V1_aegis_logo%202.png</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -6043,7 +6043,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>668e66804b755826842e2740</t>
+          <t>668c092b30b0b830ec5cebea</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -6057,7 +6057,7 @@
         </is>
       </c>
       <c r="N20" t="n">
-        <v>1720608384800</v>
+        <v>1720453419781</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -6085,10 +6085,10 @@
         </is>
       </c>
       <c r="T20" t="n">
-        <v>1720608384800</v>
+        <v>1724916846798</v>
       </c>
       <c r="U20" t="n">
-        <v>1720608384800</v>
+        <v>1720453419781</v>
       </c>
       <c r="V20" t="b">
         <v>1</v>
@@ -6108,7 +6108,7 @@
       </c>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>48b39f11-753a-464d-a75e-fdefb3d77b16</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA20" t="inlineStr">
@@ -6236,7 +6236,7 @@
       </c>
       <c r="BB20" t="inlineStr">
         <is>
-          <t>Portal.team@mobiusdtaas.ai Portal.team@mobiusdtaas.ai</t>
+          <t>Portal.team@mobiusdtaas.ai</t>
         </is>
       </c>
       <c r="BC20" t="inlineStr">
@@ -6245,16 +6245,16 @@
         </is>
       </c>
       <c r="BD20" t="n">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="BE20" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BF20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BG20" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BH20" t="inlineStr">
         <is>
@@ -6284,17 +6284,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>668c11e230b0b830ec5cec02</t>
+          <t>668c333430b0b830ec5cec60</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'TRIAL': ['668c23a430b0b830ec5cec33'], 'PLATINUM': ['668c23c230b0b830ec5cec38'], 'GOLD': ['668c23b430b0b830ec5cec35'], 'SILVER': ['668c23ab30b0b830ec5cec34']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba10ec9ef55a4cad1e1344'], 'PLATINUM': ['66ba10ecfefec82e4820d258'], 'GOLD': ['66ba10ecfefec82e4820d257'], 'SILVER': ['66ba10ec9ef55a4cad1e1345', '66d084c983d08979e96cede1']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CLink</t>
+          <t>Voxa</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -6309,17 +6309,17 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>CLink</t>
+          <t>Voxa markets government services across public and private platforms. Collaborating with Information, Public Relations, and Marketing departments, it ensures widespread awareness and engagement. Voxa leverages multiple channels to maximize the reach and impact of government programs, fostering public awareness and encouraging citizen participation in services.</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>XP</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/81b7d21a-152a-44bd-bc1b-ca3d85b03a25_$$_V1_clink%20logo%202.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/4bc5cb52-d6be-43f2-9ddc-2c6a9ec9fbed_$$_V1_Screenshot%20from%202024-07-09%2000-12-54.png</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -6334,7 +6334,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>668c11e230b0b830ec5cec01</t>
+          <t>668c333430b0b830ec5cec5f</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -6348,7 +6348,7 @@
         </is>
       </c>
       <c r="N21" t="n">
-        <v>1720455650553</v>
+        <v>1720464180041</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -6376,10 +6376,10 @@
         </is>
       </c>
       <c r="T21" t="n">
-        <v>1722328207405</v>
+        <v>1720464180041</v>
       </c>
       <c r="U21" t="n">
-        <v>1720455650553</v>
+        <v>1720464180041</v>
       </c>
       <c r="V21" t="b">
         <v>1</v>
@@ -6399,7 +6399,7 @@
       </c>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA21" t="inlineStr">
@@ -6575,17 +6575,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>66978c9c93ba7a0ac793c7b3</t>
+          <t>668e83dcc8fea21f886ddd4e</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba10e8fefec82e4820d24f'], 'PLATINUM': ['66ba10e8fefec82e4820d251'], 'GOLD': ['66ba10e89ef55a4cad1e133c'], 'SILVER': ['66ba10e8fefec82e4820d250', '66d084c883d08979e96ceddf']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Marketplace_new</t>
+          <t>Trigger Workflow</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -6600,7 +6600,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>make the bricks for that</t>
+          <t>This product is used to trigger the next workflow.</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -6608,11 +6608,7 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/2039e931-9e61-4c86-955b-0e54ce27380a_$$_V1_dummy.jpg</t>
-        </is>
-      </c>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr">
         <is>
           <t>['OTT', 'DATA CASTING']</t>
@@ -6625,7 +6621,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>66978c9c93ba7a0ac793c7b2</t>
+          <t>668e83dcc8fea21f886ddd4d</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -6639,7 +6635,7 @@
         </is>
       </c>
       <c r="N22" t="n">
-        <v>1721207964064</v>
+        <v>1720615900574</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -6667,10 +6663,10 @@
         </is>
       </c>
       <c r="T22" t="n">
-        <v>1723030415186</v>
+        <v>1721999307423</v>
       </c>
       <c r="U22" t="n">
-        <v>1721207964064</v>
+        <v>1720615900574</v>
       </c>
       <c r="V22" t="b">
         <v>1</v>
@@ -6690,7 +6686,7 @@
       </c>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA22" t="inlineStr">
@@ -6866,17 +6862,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>668c159930b0b830ec5cec0e</t>
+          <t>66976ab893ba7a0ac793c7b1</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'TRIAL': ['668c23d130b0b830ec5cec39'], 'PLATINUM': ['668c23ea30b0b830ec5cec3c'], 'GOLD': ['668c23e330b0b830ec5cec3b'], 'SILVER': ['668c23dc30b0b830ec5cec3a']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba114c9ef55a4cad1e1376'], 'PLATINUM': ['66ba114dfefec82e4820d285'], 'GOLD': ['66ba114c9ef55a4cad1e1378'], 'SILVER': ['66ba114c9ef55a4cad1e1377']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Monet</t>
+          <t>Mobius_Agent</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -6891,19 +6887,15 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Mobius</t>
+          <t xml:space="preserve">Mobius agent </t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>XP</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/1962a31e-7350-48d7-a59a-bc08161c56d8_$$_V1_monet.png</t>
-        </is>
-      </c>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr">
         <is>
           <t>['OTT', 'DATA CASTING']</t>
@@ -6916,7 +6908,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>668c159930b0b830ec5cec0d</t>
+          <t>66976ab893ba7a0ac793c7b0</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -6930,7 +6922,7 @@
         </is>
       </c>
       <c r="N23" t="n">
-        <v>1720456601053</v>
+        <v>1721199288221</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -6958,10 +6950,10 @@
         </is>
       </c>
       <c r="T23" t="n">
-        <v>1720547069960</v>
+        <v>1723530133545</v>
       </c>
       <c r="U23" t="n">
-        <v>1720456601053</v>
+        <v>1721199288221</v>
       </c>
       <c r="V23" t="b">
         <v>1</v>
@@ -6981,7 +6973,7 @@
       </c>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA23" t="inlineStr">
@@ -7131,7 +7123,7 @@
       </c>
       <c r="BH23" t="inlineStr">
         <is>
-          <t>['AD_BASED', 'Paid']</t>
+          <t>['Paid', 'AD_BASED']</t>
         </is>
       </c>
       <c r="BI23" t="inlineStr">
@@ -7157,17 +7149,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>668c161730b0b830ec5cec13</t>
+          <t>668c33e030b0b830ec5cec64</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'TRIAL': ['668c23fa30b0b830ec5cec3d'], 'PLATINUM': ['668c241d30b0b830ec5cec40'], 'GOLD': ['668c241630b0b830ec5cec3f'], 'SILVER': ['668c240330b0b830ec5cec3e']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba11369ef55a4cad1e1351'], 'PLATINUM': ['66ba1137fefec82e4820d262'], 'GOLD': ['66ba11379ef55a4cad1e1353'], 'SILVER': ['66ba11379ef55a4cad1e1352']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>BOB</t>
+          <t>Quirto</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -7182,17 +7174,17 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>BoB, or Boltzmann's Bot, is an advanced API orchestration layer designed to enhance how businesses interact with and leverage their data within the Mobius platform.</t>
+          <t>TedaaS integrates gamification, rewards, and incentives to promote government services adoption. Collaborating with nodal officers and program secretaries, it designs engaging frameworks to encourage citizen participation. TedaaS enhances user engagement and drives higher adoption rates for public programs.</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>XP</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/86fd9903-5283-4628-bb04-26b14668fa42_$$_V1_bob.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/b6c0370b-9411-40ba-b838-3c47e548f7fa_$$_V1_Screenshot%20from%202024-07-09%2000-15-38.png</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -7207,7 +7199,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>668c161730b0b830ec5cec12</t>
+          <t>668c33e030b0b830ec5cec63</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -7221,7 +7213,7 @@
         </is>
       </c>
       <c r="N24" t="n">
-        <v>1720456727756</v>
+        <v>1720464352686</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -7249,10 +7241,10 @@
         </is>
       </c>
       <c r="T24" t="n">
-        <v>1720546978864</v>
+        <v>1721998105721</v>
       </c>
       <c r="U24" t="n">
-        <v>1720456727756</v>
+        <v>1720464352686</v>
       </c>
       <c r="V24" t="b">
         <v>1</v>
@@ -7272,7 +7264,7 @@
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA24" t="inlineStr">
@@ -7448,17 +7440,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>668c0b2730b0b830ec5cebf3</t>
+          <t>6675217b72fb483cdd3be10a</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba10e99ef55a4cad1e133d'], 'PLATINUM': ['66ba10e99ef55a4cad1e133f'], 'GOLD': ['66ba10e99ef55a4cad1e133e', '66d084c883d08979e96cede0'], 'SILVER': ['66ba10e9fefec82e4820d252', '66e3d54883d08979e96cee99']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Facebook</t>
+          <t>Product_negotiation_testing3</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -7473,17 +7465,17 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Facebook is a social media platform founded by Mark Zuckerberg in 2004. It allows users to create profiles, share photos and videos, send messages, and stay connected with friends and family. Users can also join groups, follow pages, and participate in events.</t>
+          <t>weather service provider</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>XP</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/e1671c2a-85bc-49ee-9462-b2fa8bbb6fb6_$$_V1_facebook.png</t>
+          <t>https://cdn.jim-nielsen.com/ios/512/weather-2021-12-07.png</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -7498,7 +7490,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>668c0b2730b0b830ec5cebf2</t>
+          <t>6675217b72fb483cdd3be109</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -7512,7 +7504,7 @@
         </is>
       </c>
       <c r="N25" t="n">
-        <v>1720453927270</v>
+        <v>1718952315550</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -7540,10 +7532,10 @@
         </is>
       </c>
       <c r="T25" t="n">
-        <v>1721999294985</v>
+        <v>1721999006553</v>
       </c>
       <c r="U25" t="n">
-        <v>1720453927270</v>
+        <v>1718952315550</v>
       </c>
       <c r="V25" t="b">
         <v>1</v>
@@ -7563,7 +7555,7 @@
       </c>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA25" t="inlineStr">
@@ -7700,20 +7692,20 @@
         </is>
       </c>
       <c r="BD25" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BE25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BF25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BG25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BH25" t="inlineStr">
         <is>
-          <t>['AD_BASED', 'Paid']</t>
+          <t>['Paid', 'AD_BASED']</t>
         </is>
       </c>
       <c r="BI25" t="inlineStr">
@@ -7739,17 +7731,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>668c34ec30b0b830ec5cec6c</t>
+          <t>668c11e230b0b830ec5cec02</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['668c23a430b0b830ec5cec33'], 'PLATINUM': ['668c23c230b0b830ec5cec38'], 'GOLD': ['668c23b430b0b830ec5cec35'], 'SILVER': ['668c23ab30b0b830ec5cec34']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>MoScribe</t>
+          <t>CLink</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -7764,17 +7756,17 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>MoScribe streamlines citizen and organization enrollment into new services. It simplifies onboarding, making government programs accessible through the Citizen Services department. MoScribe enhances service accessibility and encourages broader participation.</t>
+          <t>CLink</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>XP</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/65e5963f-7165-46d7-b473-afd57b38304d_$$_V1_Screenshot%20from%202024-07-09%2000-19-59.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/81b7d21a-152a-44bd-bc1b-ca3d85b03a25_$$_V1_clink%20logo%202.png</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -7789,7 +7781,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>668c34ec30b0b830ec5cec6b</t>
+          <t>668c11e230b0b830ec5cec01</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -7803,7 +7795,7 @@
         </is>
       </c>
       <c r="N26" t="n">
-        <v>1720464620251</v>
+        <v>1720455650553</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -7831,10 +7823,10 @@
         </is>
       </c>
       <c r="T26" t="n">
-        <v>1720464620251</v>
+        <v>1725033135733</v>
       </c>
       <c r="U26" t="n">
-        <v>1720464620251</v>
+        <v>1720455650553</v>
       </c>
       <c r="V26" t="b">
         <v>1</v>
@@ -7854,7 +7846,7 @@
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA26" t="inlineStr">
@@ -8004,7 +7996,7 @@
       </c>
       <c r="BH26" t="inlineStr">
         <is>
-          <t>['AD_BASED', 'Paid']</t>
+          <t>['Paid', 'AD_BASED']</t>
         </is>
       </c>
       <c r="BI26" t="inlineStr">
@@ -8030,17 +8022,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>668c342030b0b830ec5cec66</t>
+          <t>668c161730b0b830ec5cec13</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['668c23fa30b0b830ec5cec3d'], 'PLATINUM': ['668c241d30b0b830ec5cec40'], 'GOLD': ['668c241630b0b830ec5cec3f'], 'SILVER': ['668c240330b0b830ec5cec3e']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CX Delight</t>
+          <t>BOB</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -8055,17 +8047,17 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>CX Delight customizes Mobius applications by region and operator, ensuring tailored user experiences. It enhances service delivery and satisfaction by providing localized interfaces. CX Delight makes government services more relevant and user-friendly for diverse communities.</t>
+          <t>BoB, or Boltzmann's Bot, is an advanced API orchestration layer designed to enhance how businesses interact with and leverage their data within the Mobius platform.</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>XP</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/1b910183-8398-4e8e-b856-e86e7195629c_$$_V1_Screenshot%20from%202024-07-09%2000-16-52.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/86fd9903-5283-4628-bb04-26b14668fa42_$$_V1_bob.png</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -8080,7 +8072,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>668c342030b0b830ec5cec65</t>
+          <t>668c161730b0b830ec5cec12</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -8094,7 +8086,7 @@
         </is>
       </c>
       <c r="N27" t="n">
-        <v>1720464416284</v>
+        <v>1720456727756</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -8122,10 +8114,10 @@
         </is>
       </c>
       <c r="T27" t="n">
-        <v>1720464416284</v>
+        <v>1723785082259</v>
       </c>
       <c r="U27" t="n">
-        <v>1720464416284</v>
+        <v>1720456727756</v>
       </c>
       <c r="V27" t="b">
         <v>1</v>
@@ -8145,7 +8137,7 @@
       </c>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA27" t="inlineStr">
@@ -8321,17 +8313,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>668c346230b0b830ec5cec68</t>
+          <t>66978c9c93ba7a0ac793c7b3</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba11379ef55a4cad1e1354'], 'PLATINUM': ['66ba11389ef55a4cad1e1356'], 'GOLD': ['66ba1138fefec82e4820d263'], 'SILVER': ['66ba11389ef55a4cad1e1355']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CMS</t>
+          <t>Marketplace_new</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -8346,17 +8338,17 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>CMS manages content for all government services, ensuring accuracy and accessibility. It supports nodal officers in maintaining up-to-date information across platforms. CMS enhances transparency and trust in government communications by centralizing content management.</t>
+          <t>make the bricks for that</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>XP</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/0cab509c-e50b-4b3c-837f-cec240314889_$$_V1_Screenshot%20from%202024-07-09%2000-17-58.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/2039e931-9e61-4c86-955b-0e54ce27380a_$$_V1_dummy.jpg</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -8371,7 +8363,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>668c346230b0b830ec5cec67</t>
+          <t>66978c9c93ba7a0ac793c7b2</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -8385,7 +8377,7 @@
         </is>
       </c>
       <c r="N28" t="n">
-        <v>1720464482647</v>
+        <v>1721207964064</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -8413,10 +8405,10 @@
         </is>
       </c>
       <c r="T28" t="n">
-        <v>1720464482647</v>
+        <v>1723030415186</v>
       </c>
       <c r="U28" t="n">
-        <v>1720464482647</v>
+        <v>1721207964064</v>
       </c>
       <c r="V28" t="b">
         <v>1</v>
@@ -8436,7 +8428,7 @@
       </c>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA28" t="inlineStr">
@@ -8586,7 +8578,7 @@
       </c>
       <c r="BH28" t="inlineStr">
         <is>
-          <t>['AD_BASED', 'Paid']</t>
+          <t>['Paid', 'AD_BASED']</t>
         </is>
       </c>
       <c r="BI28" t="inlineStr">
@@ -8612,17 +8604,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>668c111030b0b830ec5cebfe</t>
+          <t>668e80d3c8fea21f886ddd4c</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'TRIAL': ['668c227730b0b830ec5cec29'], 'PLATINUM': ['668c235130b0b830ec5cec2d'], 'GOLD': ['668c233030b0b830ec5cec2c'], 'SILVER': ['668c232830b0b830ec5cec2b']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba1140fefec82e4820d276'], 'PLATINUM': ['66ba1140fefec82e4820d279'], 'GOLD': ['66ba1140fefec82e4820d278'], 'SILVER': ['66ba1140fefec82e4820d277']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Here Here</t>
+          <t>The Base 64</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -8637,22 +8629,18 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Mobius</t>
+          <t> </t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>IP</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>https://cdn.gov-cloud.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/95b986a6-6604-4072-a812-5e850da68eac_$$_V1_here%20here.png</t>
-        </is>
-      </c>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
-          <t>['OTT', 'DATA CASTING', 'UX']</t>
+          <t>['OTT', 'DATA CASTING']</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -8662,7 +8650,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>668c111030b0b830ec5cebfd</t>
+          <t>668e80d3c8fea21f886ddd4b</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -8676,7 +8664,7 @@
         </is>
       </c>
       <c r="N29" t="n">
-        <v>1720455440057</v>
+        <v>1720615123880</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -8704,10 +8692,10 @@
         </is>
       </c>
       <c r="T29" t="n">
-        <v>1723179305674</v>
+        <v>1720615123880</v>
       </c>
       <c r="U29" t="n">
-        <v>1720455440057</v>
+        <v>1720615123880</v>
       </c>
       <c r="V29" t="b">
         <v>1</v>
@@ -8727,7 +8715,7 @@
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA29" t="inlineStr">
@@ -8870,7 +8858,7 @@
         <v>0</v>
       </c>
       <c r="BF29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG29" t="n">
         <v>0</v>
@@ -8903,17 +8891,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>66950496b8561e10d7e5d437</t>
+          <t>668c1ede30b0b830ec5cec28</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba114e9ef55a4cad1e137a'], 'PLATINUM': ['66ba114f9ef55a4cad1e137c'], 'GOLD': ['66ba114e9ef55a4cad1e137b'], 'SILVER': ['66ba114efefec82e4820d289']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ONDC</t>
+          <t>GoDaddy</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -8928,7 +8916,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Open Network for Digital Commerce, is a private non-profit Section 8 company established by the Department for Promotion of Industry and Internal Trade of Government of India to develop open e-commerce</t>
+          <t>GoDaddy is a web hosting and domain registration service. Founded in 1997, it provides a range of services including domain name registration, website building, web hosting, and online marketing tools. GoDaddy caters to individuals, small businesses, and enterprises looking to establish an online presence.</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -8936,7 +8924,11 @@
           <t>TP</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/f9c34099-facc-42f0-9b26-001ef7e2993d_$$_V1_GoDaddy.jpg</t>
+        </is>
+      </c>
       <c r="I30" t="inlineStr">
         <is>
           <t>['OTT', 'DATA CASTING']</t>
@@ -8949,7 +8941,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>66950496b8561e10d7e5d436</t>
+          <t>668c1ede30b0b830ec5cec27</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -8963,7 +8955,7 @@
         </is>
       </c>
       <c r="N30" t="n">
-        <v>1721042070451</v>
+        <v>1720458974573</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -8991,10 +8983,10 @@
         </is>
       </c>
       <c r="T30" t="n">
-        <v>1721196779341</v>
+        <v>1723552044654</v>
       </c>
       <c r="U30" t="n">
-        <v>1721042070451</v>
+        <v>1720458974573</v>
       </c>
       <c r="V30" t="b">
         <v>1</v>
@@ -9014,7 +9006,7 @@
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA30" t="inlineStr">
@@ -9164,7 +9156,7 @@
       </c>
       <c r="BH30" t="inlineStr">
         <is>
-          <t>['Paid', 'AD_BASED']</t>
+          <t>['AD_BASED', 'Paid']</t>
         </is>
       </c>
       <c r="BI30" t="inlineStr">
@@ -9190,17 +9182,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>668c35b530b0b830ec5cec70</t>
+          <t>668c09bc30b0b830ec5cebed</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['668c155630b0b830ec5cec0c'], 'PLATINUM': ['668c161b30b0b830ec5cec14'], 'GOLD': ['668c15e930b0b830ec5cec10', '668c15f330b0b830ec5cec11'], 'SILVER': ['668c15cb30b0b830ec5cec0f']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>MIB</t>
+          <t>IZAK</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -9215,17 +9207,17 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>MIB is a project management tool that integrates with systems like Jira or Asana. It evaluates sprint efforts, grooms sprints, identifies leaders and laggards, and rewards performance. MIB provides comprehensive oversight and analytics for efficient project managemen</t>
+          <t>Mobius</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>XP</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/706f1cbb-1017-43ea-908e-9c70c7da7b87_$$_V1_Screenshot%20from%202024-07-09%2000-23-35.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_232da7d6-008e-425f-9e57-fc2ae005e87d/ingestion/3c61245a-0302-434b-a192-2cb75a28cb4a_$$_V1_iZak%20logo.png</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -9240,7 +9232,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>668c35b530b0b830ec5cec6f</t>
+          <t>668c09bc30b0b830ec5cebec</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -9254,7 +9246,7 @@
         </is>
       </c>
       <c r="N31" t="n">
-        <v>1720464821212</v>
+        <v>1720453564857</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -9282,10 +9274,10 @@
         </is>
       </c>
       <c r="T31" t="n">
-        <v>1720464821212</v>
+        <v>1720459236160</v>
       </c>
       <c r="U31" t="n">
-        <v>1720464821212</v>
+        <v>1720453564857</v>
       </c>
       <c r="V31" t="b">
         <v>1</v>
@@ -9305,7 +9297,7 @@
       </c>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA31" t="inlineStr">
@@ -9433,7 +9425,7 @@
       </c>
       <c r="BB31" t="inlineStr">
         <is>
-          <t>Mobius Mobius</t>
+          <t>Portal.team@mobiusdtaas.ai</t>
         </is>
       </c>
       <c r="BC31" t="inlineStr">
@@ -9481,17 +9473,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>668c327e30b0b830ec5cec5c</t>
+          <t>668c0c8930b0b830ec5cebf5</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['668c246630b0b830ec5cec45'], 'SILVER': ['668c247130b0b830ec5cec46', '668d09218205093c726fe447']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>REVEE</t>
+          <t>OpenWeatherMap</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -9506,17 +9498,17 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Revee offers media and TV streaming services tailored for government communication. It broadcasts public service announcements, educational content, and entertainment, keeping citizens informed and engaged. This app supports government outreach efforts by providing a platform for sharing important information and engaging content with the community.</t>
+          <t>OpenWeatherMap</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>XP</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/09527cd5-74ce-4a70-ae72-10b3dad23ade_$$_V1_revee%201.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/cbedbf10-3c0b-4553-a7a6-fe2e41673a5c_$$_V1_openwethermap.png</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -9531,7 +9523,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>668c327e30b0b830ec5cec5b</t>
+          <t>668c0c8930b0b830ec5cebf4</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -9545,7 +9537,7 @@
         </is>
       </c>
       <c r="N32" t="n">
-        <v>1720463998855</v>
+        <v>1720454281566</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -9573,10 +9565,10 @@
         </is>
       </c>
       <c r="T32" t="n">
-        <v>1720528952932</v>
+        <v>1720454281566</v>
       </c>
       <c r="U32" t="n">
-        <v>1720463998855</v>
+        <v>1720454281566</v>
       </c>
       <c r="V32" t="b">
         <v>1</v>
@@ -9596,7 +9588,7 @@
       </c>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA32" t="inlineStr">
@@ -9739,7 +9731,7 @@
         <v>0</v>
       </c>
       <c r="BF32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG32" t="n">
         <v>0</v>
@@ -9772,17 +9764,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>668c1d7430b0b830ec5cec24</t>
+          <t>668c29a230b0b830ec5cec48</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba10e69ef55a4cad1e133a'], 'PLATINUM': ['66b3585bfefec82e4820d23d'], 'GOLD': ['66b358129ef55a4cad1e132a'], 'SILVER': ['66b357d09ef55a4cad1e1329']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>WhatsApp</t>
+          <t>MXaaS</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -9797,17 +9789,17 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t xml:space="preserve">WhatsApp is a messaging app that allows users to send text messages, voice messages, make voice and video calls, and share images, documents, and other media. </t>
+          <t>Marketplace as a Service</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>XP</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>https://cdn.gov-cloud.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/847a9003-06bf-4097-a90d-80936cfed99d_$$_V1_whatsapp.png</t>
+          <t>jjuuhyhg</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -9822,7 +9814,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>668c1d7430b0b830ec5cec23</t>
+          <t>668c29a230b0b830ec5cec47</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -9836,7 +9828,7 @@
         </is>
       </c>
       <c r="N33" t="n">
-        <v>1720458612036</v>
+        <v>1720461730788</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -9864,10 +9856,10 @@
         </is>
       </c>
       <c r="T33" t="n">
-        <v>1723179529824</v>
+        <v>1720529910436</v>
       </c>
       <c r="U33" t="n">
-        <v>1720458612036</v>
+        <v>1720461730788</v>
       </c>
       <c r="V33" t="b">
         <v>1</v>
@@ -9887,7 +9879,7 @@
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA33" t="inlineStr">
@@ -10030,14 +10022,14 @@
         <v>0</v>
       </c>
       <c r="BF33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BG33" t="n">
         <v>0</v>
       </c>
       <c r="BH33" t="inlineStr">
         <is>
-          <t>['Paid', 'AD_BASED']</t>
+          <t>['AD_BASED', 'Paid']</t>
         </is>
       </c>
       <c r="BI33" t="inlineStr">
@@ -10063,17 +10055,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>668c1c7730b0b830ec5cec22</t>
+          <t>668c315030b0b830ec5cec58</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba11359ef55a4cad1e134e'], 'PLATINUM': ['66ba11369ef55a4cad1e1350'], 'GOLD': ['66ba11369ef55a4cad1e134f'], 'SILVER': ['66ba1136fefec82e4820d261']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Instagram</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -10088,17 +10080,17 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Instagram is a social media platform for sharing photos and videos. Launched in 2010 and acquired by Facebook in 2012, it allows users to post visual content, follow accounts, and interact through likes, comments, and direct messages. Features include stories, reels, and various editing tools.</t>
+          <t>Mo ensures government messages reach the public effectively through diverse communication channels. It fosters transparency and engagement by keeping citizens informed about government announcements and updates. This app strengthens the relationship between the government and citizens, enhancing trust and ensuring that important information is widely disseminated.</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>XP</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/5b1c33cc-0f06-48a7-b8a7-dfe6f9d9188e_$$_V1_instagram-logo-png-transparent-background.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/0936f6ff-61bb-44ef-9223-b2ed7c0eb99a_$$_V1_mooooocolour%201.png</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -10113,7 +10105,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>668c1c7730b0b830ec5cec21</t>
+          <t>668c315030b0b830ec5cec57</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -10127,7 +10119,7 @@
         </is>
       </c>
       <c r="N34" t="n">
-        <v>1720458359494</v>
+        <v>1720463696381</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -10155,10 +10147,10 @@
         </is>
       </c>
       <c r="T34" t="n">
-        <v>1720530050313</v>
+        <v>1720530513525</v>
       </c>
       <c r="U34" t="n">
-        <v>1720458359494</v>
+        <v>1720463696381</v>
       </c>
       <c r="V34" t="b">
         <v>1</v>
@@ -10178,7 +10170,7 @@
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA34" t="inlineStr">
@@ -10328,7 +10320,7 @@
       </c>
       <c r="BH34" t="inlineStr">
         <is>
-          <t>['Paid', 'AD_BASED']</t>
+          <t>['AD_BASED', 'Paid']</t>
         </is>
       </c>
       <c r="BI34" t="inlineStr">
@@ -10354,17 +10346,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>668c113e30b0b830ec5cec00</t>
+          <t>668c349c30b0b830ec5cec6a</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'TRIAL': ['668c236b30b0b830ec5cec2e', '668c237330b0b830ec5cec2f'], 'PLATINUM': ['668c239130b0b830ec5cec32'], 'GOLD': ['668c238a30b0b830ec5cec31'], 'SILVER': ['668c237f30b0b830ec5cec30']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba1142fefec82e4820d27d'], 'PLATINUM': ['66ba11439ef55a4cad1e136c'], 'GOLD': ['66ba11439ef55a4cad1e136b'], 'SILVER': ['66ba11439ef55a4cad1e136a']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>The weather-company</t>
+          <t>AdWize1</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -10379,17 +10371,17 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Mobius</t>
+          <t>AdWize operates a programmatic ad exchange for marketing and public relations campaigns. Working with marketing departments, it optimizes ad placements to maximize message reach and impact. AdWize uses advanced targeting and analytics for efficient government campaigns.</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>XP</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/6a845d87-712e-4589-b015-427a40ef6144_$$_V1_The%20company%20wether.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/161bb23f-2b8e-4731-b246-218d9729606e_$$_V1_Screenshot%20from%202024-07-09%2000-18-56.png</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -10404,7 +10396,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>668c113e30b0b830ec5cebff</t>
+          <t>668c349c30b0b830ec5cec69</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -10418,7 +10410,7 @@
         </is>
       </c>
       <c r="N35" t="n">
-        <v>1720455486157</v>
+        <v>1720464540764</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -10446,10 +10438,10 @@
         </is>
       </c>
       <c r="T35" t="n">
-        <v>1722328270441</v>
+        <v>1723617955539</v>
       </c>
       <c r="U35" t="n">
-        <v>1720455486157</v>
+        <v>1720464540764</v>
       </c>
       <c r="V35" t="b">
         <v>1</v>
@@ -10469,7 +10461,7 @@
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA35" t="inlineStr">
@@ -10619,7 +10611,7 @@
       </c>
       <c r="BH35" t="inlineStr">
         <is>
-          <t>['Paid', 'AD_BASED']</t>
+          <t>['AD_BASED', 'Paid']</t>
         </is>
       </c>
       <c r="BI35" t="inlineStr">
@@ -10645,17 +10637,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>668c0c8930b0b830ec5cebf5</t>
+          <t>668e66804b755826842e2741</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'TRIAL': ['668c246630b0b830ec5cec45'], 'SILVER': ['668c247130b0b830ec5cec46', '668d09218205093c726fe447']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'PLATINUM': ['668e6c784b755826842e2745', '668e6cbc4b755826842e2746']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>OpenWeatherMap</t>
+          <t>PI</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -10670,7 +10662,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>OpenWeatherMap</t>
+          <t>Mobius</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -10680,7 +10672,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/cbedbf10-3c0b-4553-a7a6-fe2e41673a5c_$$_V1_openwethermap.png</t>
+          <t>jjuuhyhg</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -10695,7 +10687,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>668c0c8930b0b830ec5cebf4</t>
+          <t>668e66804b755826842e2740</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -10709,7 +10701,7 @@
         </is>
       </c>
       <c r="N36" t="n">
-        <v>1720454281566</v>
+        <v>1720608384800</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -10737,10 +10729,10 @@
         </is>
       </c>
       <c r="T36" t="n">
-        <v>1720454281566</v>
+        <v>1727083977606</v>
       </c>
       <c r="U36" t="n">
-        <v>1720454281566</v>
+        <v>1720608384800</v>
       </c>
       <c r="V36" t="b">
         <v>1</v>
@@ -10760,7 +10752,7 @@
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA36" t="inlineStr">
@@ -10888,7 +10880,7 @@
       </c>
       <c r="BB36" t="inlineStr">
         <is>
-          <t>Mobius Mobius</t>
+          <t>Portal.team@mobiusdtaas.ai Portal.team@mobiusdtaas.ai</t>
         </is>
       </c>
       <c r="BC36" t="inlineStr">
@@ -10936,17 +10928,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>668e80d3c8fea21f886ddd4c</t>
+          <t>668c0e7b30b0b830ec5cebf7</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba10ebfefec82e4820d254', '66d084c9b1dbc9702f40479e'], 'PLATINUM': ['66ba10eb9ef55a4cad1e1343'], 'GOLD': ['66ba10ebfefec82e4820d256'], 'SILVER': ['66ba10ebfefec82e4820d255', '66c8740fb1dbc9702f4045bd']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>The Base 64</t>
+          <t>WHUT - TV</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -10961,15 +10953,19 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Mobius</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>TP</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr"/>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>https://cdn.gov-cloud.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/d1c36a1d-f5bf-47ce-afbb-8811e5b51f1c_$$_V1_mhut-tv.png</t>
+        </is>
+      </c>
       <c r="I37" t="inlineStr">
         <is>
           <t>['OTT', 'DATA CASTING']</t>
@@ -10982,7 +10978,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>668e80d3c8fea21f886ddd4b</t>
+          <t>668c0e7b30b0b830ec5cebf6</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -10996,7 +10992,7 @@
         </is>
       </c>
       <c r="N37" t="n">
-        <v>1720615123880</v>
+        <v>1720454779274</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -11024,10 +11020,10 @@
         </is>
       </c>
       <c r="T37" t="n">
-        <v>1720615123880</v>
+        <v>1723184825345</v>
       </c>
       <c r="U37" t="n">
-        <v>1720615123880</v>
+        <v>1720454779274</v>
       </c>
       <c r="V37" t="b">
         <v>1</v>
@@ -11047,7 +11043,7 @@
       </c>
       <c r="Z37" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA37" t="inlineStr">
@@ -11197,7 +11193,7 @@
       </c>
       <c r="BH37" t="inlineStr">
         <is>
-          <t>['AD_BASED', 'Paid']</t>
+          <t>['Paid', 'AD_BASED']</t>
         </is>
       </c>
       <c r="BI37" t="inlineStr">
@@ -11223,17 +11219,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>668c0ac630b0b830ec5cebf1</t>
+          <t>668c346230b0b830ec5cec68</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'TRIAL': ['668c244630b0b830ec5cec42'], 'PLATINUM': ['668c243c30b0b830ec5cec41'], 'GOLD': ['668c245530b0b830ec5cec44'], 'SILVER': ['668c244d30b0b830ec5cec43']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba113bfefec82e4820d26b'], 'PLATINUM': ['66ba113cfefec82e4820d26d'], 'GOLD': ['66ba113cfefec82e4820d26c'], 'SILVER': ['66ba113b9ef55a4cad1e135c']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Kepler</t>
+          <t>CMS</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -11248,7 +11244,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Mobius</t>
+          <t>CMS manages content for all government services, ensuring accuracy and accessibility. It supports nodal officers in maintaining up-to-date information across platforms. CMS enhances transparency and trust in government communications by centralizing content management.</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -11258,7 +11254,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_232da7d6-008e-425f-9e57-fc2ae005e87d/ingestion/895e36f0-c59d-4626-9e40-62ea55a3e15d_$$_V1_Kepler.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/0cab509c-e50b-4b3c-837f-cec240314889_$$_V1_Screenshot%20from%202024-07-09%2000-17-58.png</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -11273,7 +11269,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>668c0ac630b0b830ec5cebf0</t>
+          <t>668c346230b0b830ec5cec67</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -11287,7 +11283,7 @@
         </is>
       </c>
       <c r="N38" t="n">
-        <v>1720453830929</v>
+        <v>1720464482647</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -11315,10 +11311,10 @@
         </is>
       </c>
       <c r="T38" t="n">
-        <v>1720459650985</v>
+        <v>1720464482647</v>
       </c>
       <c r="U38" t="n">
-        <v>1720453830929</v>
+        <v>1720464482647</v>
       </c>
       <c r="V38" t="b">
         <v>1</v>
@@ -11338,7 +11334,7 @@
       </c>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>232da7d6-008e-425f-9e57-fc2ae005e87d</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA38" t="inlineStr">
@@ -11466,7 +11462,7 @@
       </c>
       <c r="BB38" t="inlineStr">
         <is>
-          <t>Portal.team@mobiusdtaas.ai</t>
+          <t>Mobius Mobius</t>
         </is>
       </c>
       <c r="BC38" t="inlineStr">
@@ -11488,7 +11484,7 @@
       </c>
       <c r="BH38" t="inlineStr">
         <is>
-          <t>['Paid', 'AD_BASED']</t>
+          <t>['AD_BASED', 'Paid']</t>
         </is>
       </c>
       <c r="BI38" t="inlineStr">
@@ -11514,17 +11510,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>668c337f30b0b830ec5cec62</t>
+          <t>668c1e3530b0b830ec5cec26</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba114b9ef55a4cad1e1375'], 'PLATINUM': ['66ba114cfefec82e4820d284'], 'GOLD': ['66ba114cfefec82e4820d283'], 'SILVER': ['66ba114bfefec82e4820d282']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Marco</t>
+          <t>Gmail</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -11539,17 +11535,17 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Marco models the impact, economics, costs, and revenues of government services. Supporting Finance departments and nodal officers, it provides critical insights for financial planning and decision-making. Marco offers economic models and cost-benefit analyses, helping governments optimize resource allocation and enhance sustainability.</t>
+          <t>Gmail is a free email service developed by Google. Launched in 2004, it offers a user-friendly interface, large storage capacity, and powerful search capabilities. Gmail integrates with other Google services and supports features such as spam filtering, customizable labels, and advanced security options like two-factor authentication.</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>XP</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/3ec11f81-13ce-4d0a-a134-4d20e9f4088d_$$_V1_Screenshot%20from%202024-07-09%2000-14-03.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/80b4e199-69f5-4311-bf8e-f70368e6c537_$$_V1_Gmail-Logo-PNG-Transparent-Image.png</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -11564,7 +11560,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>668c337f30b0b830ec5cec61</t>
+          <t>668c1e3530b0b830ec5cec25</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -11578,7 +11574,7 @@
         </is>
       </c>
       <c r="N39" t="n">
-        <v>1720464255234</v>
+        <v>1720458805282</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -11606,10 +11602,10 @@
         </is>
       </c>
       <c r="T39" t="n">
-        <v>1720464255234</v>
+        <v>1724822024055</v>
       </c>
       <c r="U39" t="n">
-        <v>1720464255234</v>
+        <v>1720458805282</v>
       </c>
       <c r="V39" t="b">
         <v>1</v>
@@ -11629,7 +11625,7 @@
       </c>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA39" t="inlineStr">
@@ -11805,17 +11801,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>668c351d30b0b830ec5cec6e</t>
+          <t>668c2b8630b0b830ec5cec4c</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'PLATINUM': ['668fdb8cc8fea21f886ddd55']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>VINCI</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -11830,7 +11826,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>SMS manages citizen accounts, devices, passwords, and security. Crucial for IT departments, it ensures data integrity and seamless account management. SMS provides robust security and user-friendly tools, protecting sensitive information and maintaining trust.</t>
+          <t> </t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -11840,7 +11836,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/5b9f783c-0d91-4320-a56b-02fddc4c5f96_$$_V1_Screenshot%20from%202024-07-09%2000-21-01.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/f93bc5d6-8446-4467-a159-8a75d76f3271_$$_V1_vinci.png</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -11855,7 +11851,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>668c351d30b0b830ec5cec6d</t>
+          <t>668c2b8630b0b830ec5cec4b</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -11869,7 +11865,7 @@
         </is>
       </c>
       <c r="N40" t="n">
-        <v>1720464669346</v>
+        <v>1720462214016</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -11897,10 +11893,10 @@
         </is>
       </c>
       <c r="T40" t="n">
-        <v>1720464669346</v>
+        <v>1720547152041</v>
       </c>
       <c r="U40" t="n">
-        <v>1720464669346</v>
+        <v>1720462214016</v>
       </c>
       <c r="V40" t="b">
         <v>1</v>
@@ -11920,7 +11916,7 @@
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA40" t="inlineStr">
@@ -12063,7 +12059,7 @@
         <v>0</v>
       </c>
       <c r="BF40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG40" t="n">
         <v>0</v>
@@ -12096,17 +12092,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>668c349c30b0b830ec5cec6a</t>
+          <t>668c327e30b0b830ec5cec5c</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba113dfefec82e4820d26e', '66e3dcfdb1dbc9702f404977'], 'PLATINUM': ['66ba113efefec82e4820d271', '66e3dcfeb1dbc9702f404978'], 'GOLD': ['66ba113dfefec82e4820d270', '66e3dcfe83d08979e96cef13'], 'SILVER': ['66ba113dfefec82e4820d26f', '66e3dcfe83d08979e96cef12']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>AdWize</t>
+          <t>REVEE</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -12121,7 +12117,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>AdWize operates a programmatic ad exchange for marketing and public relations campaigns. Working with marketing departments, it optimizes ad placements to maximize message reach and impact. AdWize uses advanced targeting and analytics for efficient government campaigns.</t>
+          <t>Revee offers media and TV streaming services tailored for government communication. It broadcasts public service announcements, educational content, and entertainment, keeping citizens informed and engaged. This app supports government outreach efforts by providing a platform for sharing important information and engaging content with the community.</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -12131,7 +12127,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/161bb23f-2b8e-4731-b246-218d9729606e_$$_V1_Screenshot%20from%202024-07-09%2000-18-56.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/09527cd5-74ce-4a70-ae72-10b3dad23ade_$$_V1_revee%201.png</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -12146,7 +12142,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>668c349c30b0b830ec5cec69</t>
+          <t>668c327e30b0b830ec5cec5b</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -12160,7 +12156,7 @@
         </is>
       </c>
       <c r="N41" t="n">
-        <v>1720464540764</v>
+        <v>1720463998855</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -12188,10 +12184,10 @@
         </is>
       </c>
       <c r="T41" t="n">
-        <v>1720464540764</v>
+        <v>1720528952932</v>
       </c>
       <c r="U41" t="n">
-        <v>1720464540764</v>
+        <v>1720463998855</v>
       </c>
       <c r="V41" t="b">
         <v>1</v>
@@ -12211,7 +12207,7 @@
       </c>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA41" t="inlineStr">
@@ -12387,17 +12383,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>668c304d30b0b830ec5cec54</t>
+          <t>6694b76bc8fea21f886ddd65</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba11339ef55a4cad1e1348'], 'PLATINUM': ['66ba11339ef55a4cad1e1349', '66d084ca83d08979e96cede2'], 'GOLD': ['66ba1133fefec82e4820d25c'], 'SILVER': ['66ba1133fefec82e4820d25b']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Around</t>
+          <t>FastApi</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -12412,17 +12408,17 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Atlas manages land surveys, agriculture, and warehouses efficiently. It supports resource utilization and agricultural development by facilitating detailed land management and logistics planning. This ensures that land resources are used wisely, boosting productivity and sustainability, and supporting agricultural growth for the benefit of all citizens.</t>
+          <t>mobius</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>XP</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/e7defb56-a4ab-40d1-9f21-0386ae374f74_$$_V1_around.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/9d56fb82-a1c4-4f64-a812-6798527c541b_$$_V1_fastapiimg.png</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -12437,7 +12433,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>668c304d30b0b830ec5cec53</t>
+          <t>6694b76bc8fea21f886ddd64</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -12451,7 +12447,7 @@
         </is>
       </c>
       <c r="N42" t="n">
-        <v>1720463437594</v>
+        <v>1721022315726</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -12479,10 +12475,10 @@
         </is>
       </c>
       <c r="T42" t="n">
-        <v>1721923211699</v>
+        <v>1721299640241</v>
       </c>
       <c r="U42" t="n">
-        <v>1720463437594</v>
+        <v>1721022315726</v>
       </c>
       <c r="V42" t="b">
         <v>1</v>
@@ -12502,7 +12498,7 @@
       </c>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA42" t="inlineStr">
@@ -12652,7 +12648,7 @@
       </c>
       <c r="BH42" t="inlineStr">
         <is>
-          <t>['AD_BASED', 'Paid']</t>
+          <t>['Paid', 'AD_BASED']</t>
         </is>
       </c>
       <c r="BI42" t="inlineStr">
@@ -12678,17 +12674,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>668c0a2430b0b830ec5cebef</t>
+          <t>668c35b530b0b830ec5cec70</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba113c9ef55a4cad1e135d'], 'PLATINUM': ['66ba113d9ef55a4cad1e1360'], 'GOLD': ['66ba113c9ef55a4cad1e135f'], 'SILVER': ['66ba113c9ef55a4cad1e135e']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Tomorrow.io</t>
+          <t>MIB</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -12703,17 +12699,17 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Mobius</t>
+          <t>MIB is a project management tool that integrates with systems like Jira or Asana. It evaluates sprint efforts, grooms sprints, identifies leaders and laggards, and rewards performance. MIB provides comprehensive oversight and analytics for efficient project managemen</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>XP</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_232da7d6-008e-425f-9e57-fc2ae005e87d/ingestion/5f70aae8-e024-4b83-a450-0bdc50b26c6d_$$_V1_tomarrow.io.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/706f1cbb-1017-43ea-908e-9c70c7da7b87_$$_V1_Screenshot%20from%202024-07-09%2000-23-35.png</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -12728,7 +12724,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>668c0a2430b0b830ec5cebee</t>
+          <t>668c35b530b0b830ec5cec6f</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -12742,7 +12738,7 @@
         </is>
       </c>
       <c r="N43" t="n">
-        <v>1720453668236</v>
+        <v>1720464821212</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -12770,10 +12766,10 @@
         </is>
       </c>
       <c r="T43" t="n">
-        <v>1720459606021</v>
+        <v>1720464821212</v>
       </c>
       <c r="U43" t="n">
-        <v>1720453668236</v>
+        <v>1720464821212</v>
       </c>
       <c r="V43" t="b">
         <v>1</v>
@@ -12793,7 +12789,7 @@
       </c>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>232da7d6-008e-425f-9e57-fc2ae005e87d</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA43" t="inlineStr">
@@ -12921,7 +12917,7 @@
       </c>
       <c r="BB43" t="inlineStr">
         <is>
-          <t>Portal.team@mobiusdtaas.ai</t>
+          <t>Mobius Mobius</t>
         </is>
       </c>
       <c r="BC43" t="inlineStr">
@@ -12969,17 +12965,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>668c2fce30b0b830ec5cec52</t>
+          <t>668c304d30b0b830ec5cec54</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba1143fefec82e4820d27e'], 'PLATINUM': ['66ba11499ef55a4cad1e136f'], 'GOLD': ['66ba11499ef55a4cad1e136e'], 'SILVER': ['66ba11439ef55a4cad1e136d']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ImpressIO</t>
+          <t>Around</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -12994,7 +12990,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Impressio turns everyday objects into dynamic communication tools. It transforms highway signs into real-time incident alerts and local ad spaces into weather update platforms. This flexibility ensures citizens receive timely, relevant information through various channels, enhancing public communication and keeping the community informed and safe.</t>
+          <t>Atlas manages land surveys, agriculture, and warehouses efficiently. It supports resource utilization and agricultural development by facilitating detailed land management and logistics planning. This ensures that land resources are used wisely, boosting productivity and sustainability, and supporting agricultural growth for the benefit of all citizens.</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -13004,7 +13000,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/5b8bf081-031d-44dc-b2a4-8bb864736761_$$_V1_Frame.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/e7defb56-a4ab-40d1-9f21-0386ae374f74_$$_V1_around.png</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -13019,7 +13015,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>668c2fce30b0b830ec5cec51</t>
+          <t>668c304d30b0b830ec5cec53</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -13033,7 +13029,7 @@
         </is>
       </c>
       <c r="N44" t="n">
-        <v>1720463310070</v>
+        <v>1720463437594</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -13061,10 +13057,10 @@
         </is>
       </c>
       <c r="T44" t="n">
-        <v>1720528832394</v>
+        <v>1723785004906</v>
       </c>
       <c r="U44" t="n">
-        <v>1720463310070</v>
+        <v>1720463437594</v>
       </c>
       <c r="V44" t="b">
         <v>1</v>
@@ -13084,7 +13080,7 @@
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA44" t="inlineStr">
@@ -13260,17 +13256,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>668c1e3530b0b830ec5cec26</t>
+          <t>668c111030b0b830ec5cebfe</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['668c227730b0b830ec5cec29'], 'PLATINUM': ['668c235130b0b830ec5cec2d'], 'GOLD': ['668c233030b0b830ec5cec2c'], 'SILVER': ['668c232830b0b830ec5cec2b']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Gmail</t>
+          <t>Here Here</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -13285,22 +13281,22 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Gmail is a free email service developed by Google. Launched in 2004, it offers a user-friendly interface, large storage capacity, and powerful search capabilities. Gmail integrates with other Google services and supports features such as spam filtering, customizable labels, and advanced security options like two-factor authentication.</t>
+          <t>Mobius</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/80b4e199-69f5-4311-bf8e-f70368e6c537_$$_V1_Gmail-Logo-PNG-Transparent-Image.png</t>
+          <t>https://cdn.gov-cloud.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/95b986a6-6604-4072-a812-5e850da68eac_$$_V1_here%20here.png</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>['OTT', 'DATA CASTING']</t>
+          <t>['OTT', 'DATA CASTING', 'UX']</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -13310,7 +13306,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>668c1e3530b0b830ec5cec25</t>
+          <t>668c111030b0b830ec5cebfd</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -13324,7 +13320,7 @@
         </is>
       </c>
       <c r="N45" t="n">
-        <v>1720458805282</v>
+        <v>1720455440057</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -13352,10 +13348,10 @@
         </is>
       </c>
       <c r="T45" t="n">
-        <v>1720605407669</v>
+        <v>1723179305674</v>
       </c>
       <c r="U45" t="n">
-        <v>1720458805282</v>
+        <v>1720455440057</v>
       </c>
       <c r="V45" t="b">
         <v>1</v>
@@ -13375,7 +13371,7 @@
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA45" t="inlineStr">
@@ -13518,14 +13514,14 @@
         <v>0</v>
       </c>
       <c r="BF45" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BG45" t="n">
         <v>0</v>
       </c>
       <c r="BH45" t="inlineStr">
         <is>
-          <t>['Paid', 'AD_BASED']</t>
+          <t>['AD_BASED', 'Paid']</t>
         </is>
       </c>
       <c r="BI45" t="inlineStr">
@@ -13551,17 +13547,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>66976ab893ba7a0ac793c7b1</t>
+          <t>668c34ec30b0b830ec5cec6c</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba11399ef55a4cad1e1358'], 'PLATINUM': ['66ba113a9ef55a4cad1e1359'], 'GOLD': ['66ba113afefec82e4820d268'], 'SILVER': ['66ba113afefec82e4820d267']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Mobius_Agent</t>
+          <t>MoScribe</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -13576,15 +13572,19 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mobius agent </t>
+          <t>MoScribe streamlines citizen and organization enrollment into new services. It simplifies onboarding, making government programs accessible through the Citizen Services department. MoScribe enhances service accessibility and encourages broader participation.</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>TP</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr"/>
+          <t>XP</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/65e5963f-7165-46d7-b473-afd57b38304d_$$_V1_Screenshot%20from%202024-07-09%2000-19-59.png</t>
+        </is>
+      </c>
       <c r="I46" t="inlineStr">
         <is>
           <t>['OTT', 'DATA CASTING']</t>
@@ -13597,7 +13597,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>66976ab893ba7a0ac793c7b0</t>
+          <t>668c34ec30b0b830ec5cec6b</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -13611,7 +13611,7 @@
         </is>
       </c>
       <c r="N46" t="n">
-        <v>1721199288221</v>
+        <v>1720464620251</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -13639,10 +13639,10 @@
         </is>
       </c>
       <c r="T46" t="n">
-        <v>1722939257717</v>
+        <v>1720464620251</v>
       </c>
       <c r="U46" t="n">
-        <v>1721199288221</v>
+        <v>1720464620251</v>
       </c>
       <c r="V46" t="b">
         <v>1</v>
@@ -13662,7 +13662,7 @@
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA46" t="inlineStr">
@@ -13838,17 +13838,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>668c2b8630b0b830ec5cec4c</t>
+          <t>668c159930b0b830ec5cec0e</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {'PLATINUM': ['668fdb8cc8fea21f886ddd55']}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['668c23d130b0b830ec5cec39'], 'PLATINUM': ['668c23ea30b0b830ec5cec3c'], 'GOLD': ['668c23e330b0b830ec5cec3b'], 'SILVER': ['668c23dc30b0b830ec5cec3a']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>VINCI</t>
+          <t>Monet</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -13863,7 +13863,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Mobius</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -13873,7 +13873,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/f93bc5d6-8446-4467-a159-8a75d76f3271_$$_V1_vinci.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/1962a31e-7350-48d7-a59a-bc08161c56d8_$$_V1_monet.png</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -13888,7 +13888,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>668c2b8630b0b830ec5cec4b</t>
+          <t>668c159930b0b830ec5cec0d</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -13902,7 +13902,7 @@
         </is>
       </c>
       <c r="N47" t="n">
-        <v>1720462214016</v>
+        <v>1720456601053</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -13930,10 +13930,10 @@
         </is>
       </c>
       <c r="T47" t="n">
-        <v>1720547152041</v>
+        <v>1720547069960</v>
       </c>
       <c r="U47" t="n">
-        <v>1720462214016</v>
+        <v>1720456601053</v>
       </c>
       <c r="V47" t="b">
         <v>1</v>
@@ -13953,7 +13953,7 @@
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA47" t="inlineStr">
@@ -14129,17 +14129,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>668c31fd30b0b830ec5cec5a</t>
+          <t>668c351d30b0b830ec5cec6e</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba1141fefec82e4820d27b'], 'PLATINUM': ['66ba1142fefec82e4820d27c'], 'GOLD': ['66ba11429ef55a4cad1e1369'], 'SILVER': ['66ba11429ef55a4cad1e1368']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>HearHere</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -14154,7 +14154,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Hear, Here excels in marketing and public relations, ensuring citizens are aware of government services and benefits. It enhances the visibility and outreach of government programs through strategic communication efforts. This app keeps citizens informed and engaged, making government initiatives accessible and well-publicized</t>
+          <t>SMS manages citizen accounts, devices, passwords, and security. Crucial for IT departments, it ensures data integrity and seamless account management. SMS provides robust security and user-friendly tools, protecting sensitive information and maintaining trust.</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -14164,7 +14164,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>https://cdn.gov-cloud.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/6804a1a8-2a92-4bde-88f4-56afb61ccae0_$$_V1_here%20here.png</t>
+          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/5b9f783c-0d91-4320-a56b-02fddc4c5f96_$$_V1_Screenshot%20from%202024-07-09%2000-21-01.png</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -14179,7 +14179,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>668c31fd30b0b830ec5cec59</t>
+          <t>668c351d30b0b830ec5cec6d</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -14193,7 +14193,7 @@
         </is>
       </c>
       <c r="N48" t="n">
-        <v>1720463869655</v>
+        <v>1720464669346</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -14221,10 +14221,10 @@
         </is>
       </c>
       <c r="T48" t="n">
-        <v>1723179358214</v>
+        <v>1720464669346</v>
       </c>
       <c r="U48" t="n">
-        <v>1720463869655</v>
+        <v>1720464669346</v>
       </c>
       <c r="V48" t="b">
         <v>1</v>
@@ -14244,7 +14244,7 @@
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA48" t="inlineStr">
@@ -14420,17 +14420,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>668c1ede30b0b830ec5cec28</t>
+          <t>668c13be30b0b830ec5cec07</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba10e69ef55a4cad1e133a', '66c87858b1dbc9702f4045f8', '66d084c7b1dbc9702f40479c', '66d084cab1dbc9702f4047a0'], 'PLATINUM': ['66ba10e7fefec82e4820d24e'], 'GOLD': ['66ba10e7fefec82e4820d24d'], 'SILVER': ['66ba10e79ef55a4cad1e133b', '66c895a983d08979e96ced9d', '66c8974d83d08979e96ced9e']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>GoDaddy</t>
+          <t>Here Maps</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -14445,7 +14445,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>GoDaddy is a web hosting and domain registration service. Founded in 1997, it provides a range of services including domain name registration, website building, web hosting, and online marketing tools. GoDaddy caters to individuals, small businesses, and enterprises looking to establish an online presence.</t>
+          <t>Engagements</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -14455,7 +14455,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>https://cdn.mobiusdtaas.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/f9c34099-facc-42f0-9b26-001ef7e2993d_$$_V1_GoDaddy.jpg</t>
+          <t>https://cdn.gov-cloud.ai//_3037df6b-a4a5-4156-a128-d0e7da39c078/ingestion/3acd11c3-50a8-423b-87e3-feed87f1cd7e_$$_V1_here%20maps.png</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -14470,7 +14470,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>668c1ede30b0b830ec5cec27</t>
+          <t>668c13be30b0b830ec5cec06</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -14484,7 +14484,7 @@
         </is>
       </c>
       <c r="N49" t="n">
-        <v>1720458974573</v>
+        <v>1720456126864</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -14512,10 +14512,10 @@
         </is>
       </c>
       <c r="T49" t="n">
-        <v>1721802932803</v>
+        <v>1723179338157</v>
       </c>
       <c r="U49" t="n">
-        <v>1720458974573</v>
+        <v>1720456126864</v>
       </c>
       <c r="V49" t="b">
         <v>1</v>
@@ -14535,7 +14535,7 @@
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA49" t="inlineStr">
@@ -14685,7 +14685,7 @@
       </c>
       <c r="BH49" t="inlineStr">
         <is>
-          <t>['AD_BASED', 'Paid']</t>
+          <t>['Paid', 'AD_BASED']</t>
         </is>
       </c>
       <c r="BI49" t="inlineStr">
@@ -14711,17 +14711,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>669e35e799f8b31c3e515fc4</t>
+          <t>669603f575f6360d5ce33b02</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba1150fefec82e4820d28b'], 'PLATINUM': ['66ba1151fefec82e4820d28c'], 'GOLD': ['66ba11509ef55a4cad1e1381'], 'SILVER': ['66ba11509ef55a4cad1e1380']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Revee Channel Data</t>
+          <t>FastApi</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -14736,15 +14736,19 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t xml:space="preserve">channel data </t>
+          <t>mobius</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>XP</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr"/>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>https://cdn.mobiusdtaas.ai//_2cf76e5f-26ad-4f2c-bccc-f4bc1e7bfb64/ingestion/d255fdff-6ff6-4304-b581-1a087e26e0f7_$$_V1_fastapiimg.png</t>
+        </is>
+      </c>
       <c r="I50" t="inlineStr">
         <is>
           <t>['OTT', 'DATA CASTING']</t>
@@ -14757,7 +14761,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>669e35e799f8b31c3e515fc3</t>
+          <t>669603f575f6360d5ce33b01</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -14771,7 +14775,7 @@
         </is>
       </c>
       <c r="N50" t="n">
-        <v>1721644518752</v>
+        <v>1721107445543</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -14799,10 +14803,10 @@
         </is>
       </c>
       <c r="T50" t="n">
-        <v>1721644518752</v>
+        <v>1721107445543</v>
       </c>
       <c r="U50" t="n">
-        <v>1721644518752</v>
+        <v>1721107445543</v>
       </c>
       <c r="V50" t="b">
         <v>1</v>
@@ -14822,7 +14826,7 @@
       </c>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>3037df6b-a4a5-4156-a128-d0e7da39c078</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA50" t="inlineStr">
@@ -14950,7 +14954,7 @@
       </c>
       <c r="BB50" t="inlineStr">
         <is>
-          <t>Mobius Mobius</t>
+          <t>Aidtaas Aidtaas</t>
         </is>
       </c>
       <c r="BC50" t="inlineStr">
@@ -14998,17 +15002,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>669603f575f6360d5ce33b02</t>
+          <t>669e35e799f8b31c3e515fc4</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>{'rateCardIds': {}, 'defaultRatecardId': None}</t>
+          <t>{'rateCardIds': {'TRIAL': ['66ba114f9ef55a4cad1e137d'], 'PLATINUM': ['66ba1150fefec82e4820d28a'], 'GOLD': ['66ba114f9ef55a4cad1e137f'], 'SILVER': ['66ba114f9ef55a4cad1e137e']}, 'defaultRatecardId': None}</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>FastApi</t>
+          <t>Revee Channel Data</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -15023,19 +15027,15 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>mobius</t>
+          <t xml:space="preserve">channel data </t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>TP</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>https://cdn.mobiusdtaas.ai//_2cf76e5f-26ad-4f2c-bccc-f4bc1e7bfb64/ingestion/d255fdff-6ff6-4304-b581-1a087e26e0f7_$$_V1_fastapiimg.png</t>
-        </is>
-      </c>
+          <t>XP</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr"/>
       <c r="I51" t="inlineStr">
         <is>
           <t>['OTT', 'DATA CASTING']</t>
@@ -15048,7 +15048,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>669603f575f6360d5ce33b01</t>
+          <t>669e35e799f8b31c3e515fc3</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -15062,7 +15062,7 @@
         </is>
       </c>
       <c r="N51" t="n">
-        <v>1721107445543</v>
+        <v>1721644518752</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -15090,10 +15090,10 @@
         </is>
       </c>
       <c r="T51" t="n">
-        <v>1721107445543</v>
+        <v>1721644518752</v>
       </c>
       <c r="U51" t="n">
-        <v>1721107445543</v>
+        <v>1721644518752</v>
       </c>
       <c r="V51" t="b">
         <v>1</v>
@@ -15113,7 +15113,7 @@
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>2cf76e5f-26ad-4f2c-bccc-f4bc1e7bfb64</t>
+          <t>7c2a0cc5-6988-4999-8f6d-482363482eef</t>
         </is>
       </c>
       <c r="AA51" t="inlineStr">
@@ -15241,7 +15241,7 @@
       </c>
       <c r="BB51" t="inlineStr">
         <is>
-          <t>Aidtaas Aidtaas</t>
+          <t>Mobius Mobius</t>
         </is>
       </c>
       <c r="BC51" t="inlineStr">

</xml_diff>